<commit_message>
Todo era una mentira.
</commit_message>
<xml_diff>
--- a/Trabajo.xlsx
+++ b/Trabajo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BibliotecasUC\Documents\GitHub\Cesartoteles.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2753443C-F58D-4867-AF17-CC9997831591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED13DA6-036F-4960-92B4-BEE402C4012C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{CE01184F-E627-48DA-BF17-C376AA0D9CB6}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>